<commit_message>
ultimos cambios de sprint
</commit_message>
<xml_diff>
--- a/reports/pagos.xlsx
+++ b/reports/pagos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>PARTICIPANTE</t>
   </si>
@@ -32,6 +32,45 @@
   </si>
   <si>
     <t>VALOR CANCELADO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramírez Buendía Daniel Sebastián </t>
+  </si>
+  <si>
+    <t>1714108568</t>
+  </si>
+  <si>
+    <t>156341</t>
+  </si>
+  <si>
+    <t>$ 200</t>
+  </si>
+  <si>
+    <t>Chasiloa Páez Mirian Amparo</t>
+  </si>
+  <si>
+    <t>1003834627001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yithos</t>
+  </si>
+  <si>
+    <t>45872</t>
+  </si>
+  <si>
+    <t>$ 110</t>
+  </si>
+  <si>
+    <t>Quiguango Rivera Alisson Lorena</t>
+  </si>
+  <si>
+    <t>1003834627</t>
+  </si>
+  <si>
+    <t>555</t>
+  </si>
+  <si>
+    <t>$ 100</t>
   </si>
 </sst>
 </file>
@@ -67,8 +106,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
@@ -442,6 +482,75 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>165843</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>44141</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>45872</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>44144</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>666</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44137</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>